<commit_message>
Aggiunto test per CN43N
</commit_message>
<xml_diff>
--- a/Solution/FilesEditor.Tests/TestFiles/SourceFiles/CN43N.xlsx
+++ b/Solution/FilesEditor.Tests/TestFiles/SourceFiles/CN43N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fperrino\Desktop\KPI UT_LAVORO_LEFO\Files\File Originali\SuperDettagli\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Lefo\Dev\3 GDPptGenerator\Solution\FilesEditor.Tests\TestFiles\SourceFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABF803B-1292-43FF-86F1-1D19AFEF2BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EB75E79-E678-4CC6-9FC1-5D03BE7D91B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="24">
   <si>
     <t>Level</t>
   </si>
@@ -254,9 +254,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -266,10 +263,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -553,23 +553,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="V11" sqref="V11:V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -644,59 +648,501 @@
       <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="10">
         <v>42369</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>17</v>
       </c>
       <c r="L2" s="5"/>
-      <c r="M2" s="6">
+      <c r="M2" s="10">
         <v>42145</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="10">
-        <v>42369</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="9"/>
-      <c r="M3" s="10">
-        <v>42145</v>
-      </c>
-      <c r="N3" s="11" t="s">
+      <c r="I3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="11">
+        <f>J2+1</f>
+        <v>42370</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="11">
+        <f t="shared" ref="M3:M13" si="0">M2+1</f>
+        <v>42146</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="10">
+        <f t="shared" ref="J4:J13" si="1">J3+1</f>
+        <v>42371</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="10">
+        <f t="shared" si="0"/>
+        <v>42147</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="1"/>
+        <v>42372</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L5" s="8"/>
+      <c r="M5" s="11">
+        <f t="shared" si="0"/>
+        <v>42148</v>
+      </c>
+      <c r="N5" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" si="1"/>
+        <v>42373</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="10">
+        <f t="shared" si="0"/>
+        <v>42149</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="11">
+        <f t="shared" si="1"/>
+        <v>42374</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="11">
+        <f t="shared" si="0"/>
+        <v>42150</v>
+      </c>
+      <c r="N7" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
+        <v>42375</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="10">
+        <f t="shared" si="0"/>
+        <v>42151</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="11">
+        <f t="shared" si="1"/>
+        <v>42376</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="11">
+        <f t="shared" si="0"/>
+        <v>42152</v>
+      </c>
+      <c r="N9" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="1"/>
+        <v>42377</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="10">
+        <f t="shared" si="0"/>
+        <v>42153</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" s="11">
+        <f t="shared" si="1"/>
+        <v>42378</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="11">
+        <f t="shared" si="0"/>
+        <v>42154</v>
+      </c>
+      <c r="N11" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
+        <v>42379</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="10">
+        <f t="shared" si="0"/>
+        <v>42155</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="11">
+        <f t="shared" si="1"/>
+        <v>42380</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L13" s="8"/>
+      <c r="M13" s="11">
+        <f t="shared" si="0"/>
+        <v>42156</v>
+      </c>
+      <c r="N13" s="9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>